<commit_message>
Freeze header row and county column
</commit_message>
<xml_diff>
--- a/CommonFiles/COPsyncPresence.xlsx
+++ b/CommonFiles/COPsyncPresence.xlsx
@@ -1935,7 +1935,10 @@
   <dimension ref="A1:E255"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>